<commit_message>
basic animation and color
</commit_message>
<xml_diff>
--- a/beauty/data/gg_gdp_s.xlsx
+++ b/beauty/data/gg_gdp_s.xlsx
@@ -144,15 +144,6 @@
     <t>United States,2014</t>
   </si>
   <si>
-    <t>Columbia,2006</t>
-  </si>
-  <si>
-    <t>Columbia,2010</t>
-  </si>
-  <si>
-    <t>Columbia,2014</t>
-  </si>
-  <si>
     <t>Chile,2006</t>
   </si>
   <si>
@@ -210,6 +201,18 @@
   </si>
   <si>
     <t>rank_rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Colombia,2006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Colombia,2010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Colombia,2014</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -619,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -694,13 +697,13 @@
         <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="V1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="W1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:23">
@@ -2217,7 +2220,7 @@
     </row>
     <row r="23" spans="1:23">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="B23">
         <v>0.76</v>
@@ -2289,7 +2292,7 @@
     </row>
     <row r="24" spans="1:23">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="B24">
         <v>0.55000000000000004</v>
@@ -2361,7 +2364,7 @@
     </row>
     <row r="25" spans="1:23">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B25">
         <v>0.72</v>
@@ -2433,7 +2436,7 @@
     </row>
     <row r="26" spans="1:23">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B26">
         <v>0.52</v>
@@ -2505,7 +2508,7 @@
     </row>
     <row r="27" spans="1:23">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B27">
         <v>0.6</v>
@@ -2577,7 +2580,7 @@
     </row>
     <row r="28" spans="1:23">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B28">
         <v>0.69</v>
@@ -2649,7 +2652,7 @@
     </row>
     <row r="29" spans="1:23">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B29">
         <v>0.84</v>
@@ -2721,7 +2724,7 @@
     </row>
     <row r="30" spans="1:23">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B30">
         <v>0.88</v>
@@ -2793,7 +2796,7 @@
     </row>
     <row r="31" spans="1:23">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B31">
         <v>0.84</v>
@@ -2865,7 +2868,7 @@
     </row>
     <row r="32" spans="1:23">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B32">
         <v>0.92</v>
@@ -2880,7 +2883,7 @@
         <v>0.16</v>
       </c>
       <c r="F32" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G32">
         <v>0.75</v>
@@ -2937,7 +2940,7 @@
     </row>
     <row r="33" spans="1:23">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B33">
         <v>0.88</v>
@@ -3009,7 +3012,7 @@
     </row>
     <row r="34" spans="1:23">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B34">
         <v>0.96</v>
@@ -3081,7 +3084,7 @@
     </row>
     <row r="35" spans="1:23">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B35">
         <v>0.66</v>
@@ -3153,7 +3156,7 @@
     </row>
     <row r="36" spans="1:23">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B36">
         <v>0.73</v>
@@ -3225,7 +3228,7 @@
     </row>
     <row r="37" spans="1:23">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B37">
         <v>0.75</v>
@@ -3297,7 +3300,7 @@
     </row>
     <row r="38" spans="1:23">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B38">
         <v>0.41</v>
@@ -3369,7 +3372,7 @@
     </row>
     <row r="39" spans="1:23">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B39">
         <v>0.42</v>
@@ -3384,7 +3387,7 @@
         <v>0.03</v>
       </c>
       <c r="F39" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G39">
         <v>0.68</v>
@@ -3441,7 +3444,7 @@
     </row>
     <row r="40" spans="1:23">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B40">
         <v>0.36</v>
@@ -3453,10 +3456,10 @@
         <v>0.24</v>
       </c>
       <c r="E40" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F40" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G40">
         <v>0.68</v>

</xml_diff>